<commit_message>
setting up nowcasting from automatic download of eber data
</commit_message>
<xml_diff>
--- a/Aggregations/1. Nowcasting electricity.xlsx
+++ b/Aggregations/1. Nowcasting electricity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\Documents\GitHub\desktop-tutorial\ExtremesBEV\Aggregations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\ExtremesBEV\Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE7B226-1CA8-49C8-807A-F0C42C201364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE805E9-DD62-4B3E-89AD-A6B254156AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="777">
   <si>
     <t>Aggregation</t>
   </si>
@@ -2353,6 +2353,9 @@
   </si>
   <si>
     <t>Other Renewables</t>
+  </si>
+  <si>
+    <t>Electricity</t>
   </si>
 </sst>
 </file>
@@ -2722,582 +2725,582 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="114.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="114.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
@@ -3305,7 +3308,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
@@ -3313,7 +3316,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
@@ -3321,7 +3324,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
@@ -3329,7 +3332,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
@@ -3337,7 +3340,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
@@ -3345,7 +3348,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
@@ -3353,7 +3356,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
@@ -3361,7 +3364,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
@@ -3369,7 +3372,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
@@ -3385,7 +3388,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
@@ -3393,202 +3396,202 @@
         <v>772</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>164</v>
       </c>
@@ -3602,1053 +3605,1053 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43:B54"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="120.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="120.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B43" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>205</v>
       </c>
       <c r="B44" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>206</v>
       </c>
       <c r="B45" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B46" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B47" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B48" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B49" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>211</v>
       </c>
       <c r="B50" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B51" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>213</v>
       </c>
       <c r="B52" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>214</v>
       </c>
       <c r="B53" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B54" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>354</v>
       </c>
@@ -4664,49 +4667,49 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>362</v>
       </c>
@@ -4722,1759 +4725,1759 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>712</v>
       </c>
@@ -6490,39 +6493,39 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>718</v>
       </c>
@@ -6538,249 +6541,249 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>766</v>
       </c>

</xml_diff>